<commit_message>
Update prices, add 3D models, update AstriOS
</commit_message>
<xml_diff>
--- a/Docs/prices.xlsx
+++ b/Docs/prices.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Наименование</t>
   </si>
@@ -41,38 +42,59 @@
     <t>Оптовая цена в Китае, руб</t>
   </si>
   <si>
-    <t>Двигатель 24BYJ48</t>
-  </si>
-  <si>
-    <t>Радиомодуль nrf24l01</t>
-  </si>
-  <si>
-    <t>Радиомодуль nrf24l01 +</t>
-  </si>
-  <si>
-    <t>Адаптер для nrf24l01</t>
-  </si>
-  <si>
     <t>Итого:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Драйвер двигателя l293d</t>
-    </r>
+    <t>Arduino nano</t>
+  </si>
+  <si>
+    <t>Wemos d1 mini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Модуль SD карты </t>
+  </si>
+  <si>
+    <t>SD карта</t>
+  </si>
+  <si>
+    <t>Драйвер двигателя ULN2003</t>
+  </si>
+  <si>
+    <t>Шаговый двигатель 28byj-48</t>
+  </si>
+  <si>
+    <t>Модуль реального времени DS1307</t>
+  </si>
+  <si>
+    <t>Сервопривод mg90s</t>
+  </si>
+  <si>
+    <t>Пьезо-пищалка</t>
+  </si>
+  <si>
+    <t>Дисплей Nextion</t>
+  </si>
+  <si>
+    <t>Сенсорная кнопка TTP223</t>
+  </si>
+  <si>
+    <t>Стилус</t>
+  </si>
+  <si>
+    <t>Замок</t>
+  </si>
+  <si>
+    <t>Переключатель</t>
+  </si>
+  <si>
+    <t>Arduino mega 2560 pro mini</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,13 +242,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -904,13 +919,13 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
@@ -940,16 +955,16 @@
     </row>
     <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>152</v>
+        <v>1021</v>
       </c>
       <c r="D2" s="1">
-        <v>12.5</v>
+        <v>468.5</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -958,16 +973,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>250</v>
+        <v>284.05</v>
       </c>
       <c r="D3" s="1">
-        <v>150</v>
+        <v>107.5</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -976,16 +991,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>170</v>
+        <v>270.75799999999998</v>
       </c>
       <c r="D4" s="1">
-        <v>47.25</v>
+        <v>119.35</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -994,16 +1009,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>262</v>
+        <v>2355</v>
       </c>
       <c r="D5" s="1">
-        <v>130</v>
+        <v>800</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1015,13 +1030,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="D6" s="1">
-        <v>25</v>
+        <v>27.94</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1029,147 +1044,204 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="1">
+        <v>250</v>
+      </c>
+      <c r="D7" s="1">
+        <v>83.8</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>240</v>
+      </c>
+      <c r="D8" s="1">
+        <v>92.78</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1">
+        <v>32.380000000000003</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="1">
+        <v>97</v>
+      </c>
+      <c r="D10" s="1">
+        <v>34.92</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="1">
+        <v>160</v>
+      </c>
+      <c r="D11" s="1">
+        <v>124.56</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="1">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="1">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1">
+        <v>12</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="1">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="C15" s="1">
+        <v>92.2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>51.3</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="C16" s="1">
+        <v>137</v>
+      </c>
+      <c r="D16" s="1">
+        <v>32.380000000000003</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="1">
         <f ca="1">SUMPRODUCT(B2:INDIRECT(ADDRESS(ROW()-1,2)),C2:INDIRECT(ADDRESS(ROW()-1,3)))</f>
-        <v>1350</v>
+        <v>5426.0079999999998</v>
       </c>
       <c r="D17" s="1">
         <f ca="1">SUMPRODUCT(B2:INDIRECT(ADDRESS(ROW()-1,2)),D2:INDIRECT(ADDRESS(ROW()-1,4)))</f>
-        <v>552.25</v>
+        <v>2124.37</v>
       </c>
       <c r="E17" s="1">
         <f ca="1">SUMPRODUCT(B2:INDIRECT(ADDRESS(ROW()-1,2)),E2:INDIRECT(ADDRESS(ROW()-1,5)))</f>
         <v>0</v>
       </c>
-      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>

</xml_diff>